<commit_message>
Revert "Update experimental results"
This reverts commit bb0575ca
</commit_message>
<xml_diff>
--- a/experiment_results/DataV2_0.5/BankAccountTP/ENABLE_NORMALIZATION/AGGREGATION_ARITHMETIC_MEAN/4wise/1Bug.xlsx
+++ b/experiment_results/DataV2_0.5/BankAccountTP/ENABLE_NORMALIZATION/AGGREGATION_ARITHMETIC_MEAN/4wise/1Bug.xlsx
@@ -765,13 +765,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -803,19 +803,19 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>3.947368421052631</v>
+        <v>13.1578947368421</v>
       </c>
       <c r="E3">
         <v>40</v>
       </c>
       <c r="F3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3">
-        <v>14.47368421052632</v>
+        <v>15.78947368421053</v>
       </c>
       <c r="H3">
         <v>21</v>
@@ -1449,10 +1449,10 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D20">
-        <v>10.52631578947368</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E20">
         <v>26</v>
@@ -2136,10 +2136,10 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>10.52631578947368</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E38">
         <v>26</v>
@@ -2250,10 +2250,10 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41">
-        <v>13.1578947368421</v>
+        <v>10.52631578947368</v>
       </c>
       <c r="E41">
         <v>14</v>
@@ -2364,19 +2364,19 @@
         <v>16</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D44">
-        <v>3.947368421052631</v>
+        <v>13.1578947368421</v>
       </c>
       <c r="E44">
         <v>42</v>
       </c>
       <c r="F44">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G44">
-        <v>5.263157894736842</v>
+        <v>15.78947368421053</v>
       </c>
       <c r="H44">
         <v>22</v>
@@ -3599,13 +3599,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -5806,10 +5806,10 @@
         <v>27</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D60">
-        <v>6.578947368421052</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E60">
         <v>26</v>
@@ -6433,13 +6433,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -8032,10 +8032,10 @@
         <v>16</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>2.631578947368421</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E44">
         <v>42</v>
@@ -8640,19 +8640,19 @@
         <v>27</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D60">
-        <v>6.578947368421052</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E60">
         <v>26</v>
       </c>
       <c r="F60">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G60">
-        <v>6.578947368421052</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="H60">
         <v>5</v>
@@ -9267,13 +9267,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -9457,19 +9457,19 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>64.47368421052632</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>64.47368421052632</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H7">
         <v>57</v>
@@ -9913,19 +9913,19 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>64.47368421052632</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>64.47368421052632</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H19">
         <v>57</v>
@@ -9951,19 +9951,19 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D20">
-        <v>21.05263157894737</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E20">
         <v>26</v>
       </c>
       <c r="F20">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G20">
-        <v>53.94736842105263</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H20">
         <v>68</v>
@@ -10258,19 +10258,19 @@
         <v>24</v>
       </c>
       <c r="C28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="H28">
         <v>60</v>
@@ -10296,19 +10296,19 @@
         <v>48</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D29">
-        <v>2.631578947368421</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E29">
         <v>29</v>
       </c>
       <c r="F29">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G29">
-        <v>5.263157894736842</v>
+        <v>9.210526315789473</v>
       </c>
       <c r="H29">
         <v>6</v>
@@ -10562,10 +10562,10 @@
         <v>69</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>2.631578947368421</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E36">
         <v>34</v>
@@ -10638,19 +10638,19 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D38">
-        <v>21.05263157894737</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E38">
         <v>26</v>
       </c>
       <c r="F38">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G38">
-        <v>53.94736842105263</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H38">
         <v>68</v>
@@ -10828,10 +10828,10 @@
         <v>37</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D43">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E43">
         <v>12</v>
@@ -10904,19 +10904,19 @@
         <v>57</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E45">
         <v>24</v>
       </c>
       <c r="F45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G45">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H45">
         <v>3</v>
@@ -11857,19 +11857,19 @@
         <v>85</v>
       </c>
       <c r="C70">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D70">
-        <v>48.68421052631579</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="G70">
-        <v>48.68421052631579</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="H70">
         <v>37</v>
@@ -12101,13 +12101,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -12291,19 +12291,19 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>64.47368421052632</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>64.47368421052632</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H7">
         <v>57</v>
@@ -12747,19 +12747,19 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>64.47368421052632</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>64.47368421052632</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H19">
         <v>57</v>
@@ -12785,19 +12785,19 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D20">
-        <v>21.05263157894737</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E20">
         <v>26</v>
       </c>
       <c r="F20">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G20">
-        <v>53.94736842105263</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H20">
         <v>68</v>
@@ -13092,19 +13092,19 @@
         <v>24</v>
       </c>
       <c r="C28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="H28">
         <v>60</v>
@@ -13130,19 +13130,19 @@
         <v>48</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D29">
-        <v>2.631578947368421</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E29">
         <v>29</v>
       </c>
       <c r="F29">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G29">
-        <v>5.263157894736842</v>
+        <v>9.210526315789473</v>
       </c>
       <c r="H29">
         <v>6</v>
@@ -13396,10 +13396,10 @@
         <v>69</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>2.631578947368421</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E36">
         <v>34</v>
@@ -13472,19 +13472,19 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D38">
-        <v>21.05263157894737</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E38">
         <v>26</v>
       </c>
       <c r="F38">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G38">
-        <v>53.94736842105263</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H38">
         <v>68</v>
@@ -13662,10 +13662,10 @@
         <v>37</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D43">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E43">
         <v>12</v>
@@ -13738,19 +13738,19 @@
         <v>57</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E45">
         <v>24</v>
       </c>
       <c r="F45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G45">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H45">
         <v>3</v>
@@ -14691,19 +14691,19 @@
         <v>85</v>
       </c>
       <c r="C70">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D70">
-        <v>48.68421052631579</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="G70">
-        <v>48.68421052631579</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="H70">
         <v>37</v>
@@ -14935,13 +14935,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -15619,19 +15619,19 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D20">
-        <v>11.84210526315789</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E20">
         <v>26</v>
       </c>
       <c r="F20">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G20">
-        <v>13.1578947368421</v>
+        <v>17.10526315789474</v>
       </c>
       <c r="H20">
         <v>15</v>
@@ -16306,19 +16306,19 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>11.84210526315789</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E38">
         <v>26</v>
       </c>
       <c r="F38">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G38">
-        <v>13.1578947368421</v>
+        <v>17.10526315789474</v>
       </c>
       <c r="H38">
         <v>15</v>
@@ -16420,10 +16420,10 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41">
-        <v>13.1578947368421</v>
+        <v>10.52631578947368</v>
       </c>
       <c r="E41">
         <v>14</v>
@@ -17066,10 +17066,10 @@
         <v>57</v>
       </c>
       <c r="C58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D58">
-        <v>5.263157894736842</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E58">
         <v>23</v>
@@ -17769,13 +17769,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -19254,10 +19254,10 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41">
-        <v>13.1578947368421</v>
+        <v>10.52631578947368</v>
       </c>
       <c r="E41">
         <v>14</v>
@@ -19558,10 +19558,10 @@
         <v>83</v>
       </c>
       <c r="C49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>11.84210526315789</v>
+        <v>9.210526315789473</v>
       </c>
       <c r="E49">
         <v>11</v>
@@ -20603,13 +20603,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>24.05063291139241</v>
+        <v>6.329113924050633</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>19</v>
@@ -23437,13 +23437,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -23627,19 +23627,19 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>81.57894736842105</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>81.57894736842105</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H7">
         <v>70</v>
@@ -23788,10 +23788,10 @@
         <v>26</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H11">
         <v>52</v>
@@ -23969,10 +23969,10 @@
         <v>41</v>
       </c>
       <c r="C16">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>11.84210526315789</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E16">
         <v>24</v>
@@ -24083,19 +24083,19 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>81.57894736842105</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>81.57894736842105</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H19">
         <v>70</v>
@@ -24121,19 +24121,19 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D20">
-        <v>18.42105263157895</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E20">
         <v>26</v>
       </c>
       <c r="F20">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G20">
-        <v>72.36842105263158</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H20">
         <v>75</v>
@@ -24238,19 +24238,19 @@
         <v>20</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E23">
         <v>12</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H23">
         <v>34</v>
@@ -24285,10 +24285,10 @@
         <v>17</v>
       </c>
       <c r="F24">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G24">
-        <v>12.65822784810127</v>
+        <v>10.12658227848101</v>
       </c>
       <c r="H24">
         <v>47</v>
@@ -24314,19 +24314,19 @@
         <v>41</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H25">
         <v>48</v>
@@ -24428,19 +24428,19 @@
         <v>24</v>
       </c>
       <c r="C28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="H28">
         <v>70</v>
@@ -24504,19 +24504,19 @@
         <v>61</v>
       </c>
       <c r="C30">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D30">
-        <v>16.45569620253164</v>
+        <v>8.860759493670885</v>
       </c>
       <c r="E30">
         <v>32</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30">
-        <v>12.65822784810127</v>
+        <v>11.39240506329114</v>
       </c>
       <c r="H30">
         <v>55</v>
@@ -24656,19 +24656,19 @@
         <v>57</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E34">
         <v>12</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H34">
         <v>36</v>
@@ -24779,10 +24779,10 @@
         <v>24</v>
       </c>
       <c r="F37">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G37">
-        <v>16.45569620253164</v>
+        <v>12.65822784810127</v>
       </c>
       <c r="H37">
         <v>47</v>
@@ -24808,19 +24808,19 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D38">
-        <v>18.42105263157895</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E38">
         <v>26</v>
       </c>
       <c r="F38">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G38">
-        <v>72.36842105263158</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H38">
         <v>75</v>
@@ -24931,10 +24931,10 @@
         <v>14</v>
       </c>
       <c r="F41">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G41">
-        <v>13.1578947368421</v>
+        <v>11.84210526315789</v>
       </c>
       <c r="H41">
         <v>49</v>
@@ -24960,19 +24960,19 @@
         <v>22</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H42">
         <v>28</v>
@@ -24998,19 +24998,19 @@
         <v>37</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D43">
-        <v>9.210526315789473</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E43">
         <v>12</v>
       </c>
       <c r="F43">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G43">
-        <v>14.47368421052632</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="H43">
         <v>57</v>
@@ -25074,10 +25074,10 @@
         <v>57</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E45">
         <v>24</v>
@@ -25226,10 +25226,10 @@
         <v>83</v>
       </c>
       <c r="C49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>11.84210526315789</v>
+        <v>9.210526315789473</v>
       </c>
       <c r="E49">
         <v>11</v>
@@ -25273,10 +25273,10 @@
         <v>2</v>
       </c>
       <c r="F50">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G50">
-        <v>11.84210526315789</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H50">
         <v>47</v>
@@ -25311,10 +25311,10 @@
         <v>11</v>
       </c>
       <c r="F51">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G51">
-        <v>13.1578947368421</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H51">
         <v>34</v>
@@ -25843,10 +25843,10 @@
         <v>26</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G65">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H65">
         <v>28</v>
@@ -25960,10 +25960,10 @@
         <v>26</v>
       </c>
       <c r="F68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G68">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H68">
         <v>28</v>
@@ -26027,19 +26027,19 @@
         <v>85</v>
       </c>
       <c r="C70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="G70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="H70">
         <v>54</v>
@@ -26271,13 +26271,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -28060,10 +28060,10 @@
         <v>83</v>
       </c>
       <c r="C49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>11.84210526315789</v>
+        <v>9.210526315789473</v>
       </c>
       <c r="E49">
         <v>11</v>
@@ -28402,19 +28402,19 @@
         <v>57</v>
       </c>
       <c r="C58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D58">
-        <v>5.263157894736842</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E58">
         <v>23</v>
       </c>
       <c r="F58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G58">
-        <v>5.263157894736842</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="H58">
         <v>5</v>
@@ -28478,10 +28478,10 @@
         <v>27</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D60">
-        <v>6.578947368421052</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E60">
         <v>26</v>
@@ -29105,13 +29105,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -31312,10 +31312,10 @@
         <v>27</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D60">
-        <v>6.578947368421052</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E60">
         <v>26</v>
@@ -31939,13 +31939,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -32623,19 +32623,19 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D20">
-        <v>10.52631578947368</v>
+        <v>11.84210526315789</v>
       </c>
       <c r="E20">
         <v>26</v>
       </c>
       <c r="F20">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G20">
-        <v>11.84210526315789</v>
+        <v>13.1578947368421</v>
       </c>
       <c r="H20">
         <v>14</v>
@@ -33310,19 +33310,19 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D38">
-        <v>10.52631578947368</v>
+        <v>11.84210526315789</v>
       </c>
       <c r="E38">
         <v>26</v>
       </c>
       <c r="F38">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G38">
-        <v>11.84210526315789</v>
+        <v>13.1578947368421</v>
       </c>
       <c r="H38">
         <v>14</v>
@@ -33424,10 +33424,10 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41">
-        <v>13.1578947368421</v>
+        <v>10.52631578947368</v>
       </c>
       <c r="E41">
         <v>14</v>
@@ -33728,10 +33728,10 @@
         <v>83</v>
       </c>
       <c r="C49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>11.84210526315789</v>
+        <v>9.210526315789473</v>
       </c>
       <c r="E49">
         <v>11</v>
@@ -34773,13 +34773,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -34963,19 +34963,19 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H7">
         <v>70</v>
@@ -35124,10 +35124,10 @@
         <v>26</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H11">
         <v>52</v>
@@ -35305,10 +35305,10 @@
         <v>41</v>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>10.52631578947368</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E16">
         <v>24</v>
@@ -35419,19 +35419,19 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H19">
         <v>70</v>
@@ -35457,19 +35457,19 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D20">
-        <v>22.36842105263158</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E20">
         <v>26</v>
       </c>
       <c r="F20">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G20">
-        <v>72.36842105263158</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H20">
         <v>75</v>
@@ -35574,19 +35574,19 @@
         <v>20</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E23">
         <v>12</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H23">
         <v>34</v>
@@ -35621,10 +35621,10 @@
         <v>17</v>
       </c>
       <c r="F24">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G24">
-        <v>12.65822784810127</v>
+        <v>10.12658227848101</v>
       </c>
       <c r="H24">
         <v>47</v>
@@ -35650,19 +35650,19 @@
         <v>41</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H25">
         <v>48</v>
@@ -35764,19 +35764,19 @@
         <v>24</v>
       </c>
       <c r="C28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="H28">
         <v>70</v>
@@ -35840,19 +35840,19 @@
         <v>61</v>
       </c>
       <c r="C30">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D30">
-        <v>16.45569620253164</v>
+        <v>8.860759493670885</v>
       </c>
       <c r="E30">
         <v>32</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30">
-        <v>12.65822784810127</v>
+        <v>11.39240506329114</v>
       </c>
       <c r="H30">
         <v>55</v>
@@ -35992,19 +35992,19 @@
         <v>57</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E34">
         <v>12</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H34">
         <v>36</v>
@@ -36115,10 +36115,10 @@
         <v>24</v>
       </c>
       <c r="F37">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G37">
-        <v>16.45569620253164</v>
+        <v>12.65822784810127</v>
       </c>
       <c r="H37">
         <v>47</v>
@@ -36144,19 +36144,19 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D38">
-        <v>22.36842105263158</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E38">
         <v>26</v>
       </c>
       <c r="F38">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G38">
-        <v>72.36842105263158</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H38">
         <v>75</v>
@@ -36267,10 +36267,10 @@
         <v>14</v>
       </c>
       <c r="F41">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G41">
-        <v>14.47368421052632</v>
+        <v>11.84210526315789</v>
       </c>
       <c r="H41">
         <v>49</v>
@@ -36296,19 +36296,19 @@
         <v>22</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H42">
         <v>28</v>
@@ -36334,19 +36334,19 @@
         <v>37</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D43">
-        <v>9.210526315789473</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E43">
         <v>12</v>
       </c>
       <c r="F43">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G43">
-        <v>14.47368421052632</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="H43">
         <v>57</v>
@@ -36410,10 +36410,10 @@
         <v>57</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E45">
         <v>24</v>
@@ -36609,10 +36609,10 @@
         <v>2</v>
       </c>
       <c r="F50">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G50">
-        <v>11.84210526315789</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H50">
         <v>47</v>
@@ -36647,10 +36647,10 @@
         <v>11</v>
       </c>
       <c r="F51">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G51">
-        <v>13.1578947368421</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H51">
         <v>34</v>
@@ -37179,10 +37179,10 @@
         <v>26</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G65">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H65">
         <v>28</v>
@@ -37296,10 +37296,10 @@
         <v>26</v>
       </c>
       <c r="F68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G68">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H68">
         <v>28</v>
@@ -37363,19 +37363,19 @@
         <v>85</v>
       </c>
       <c r="C70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="G70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="H70">
         <v>54</v>
@@ -37607,13 +37607,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -37797,19 +37797,19 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H7">
         <v>70</v>
@@ -37958,10 +37958,10 @@
         <v>26</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H11">
         <v>52</v>
@@ -38139,10 +38139,10 @@
         <v>41</v>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>10.52631578947368</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E16">
         <v>24</v>
@@ -38253,19 +38253,19 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H19">
         <v>70</v>
@@ -38291,19 +38291,19 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D20">
-        <v>22.36842105263158</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E20">
         <v>26</v>
       </c>
       <c r="F20">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G20">
-        <v>72.36842105263158</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H20">
         <v>75</v>
@@ -38408,19 +38408,19 @@
         <v>20</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E23">
         <v>12</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H23">
         <v>34</v>
@@ -38455,10 +38455,10 @@
         <v>17</v>
       </c>
       <c r="F24">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G24">
-        <v>12.65822784810127</v>
+        <v>10.12658227848101</v>
       </c>
       <c r="H24">
         <v>47</v>
@@ -38484,19 +38484,19 @@
         <v>41</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H25">
         <v>48</v>
@@ -38598,19 +38598,19 @@
         <v>24</v>
       </c>
       <c r="C28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="H28">
         <v>70</v>
@@ -38674,19 +38674,19 @@
         <v>61</v>
       </c>
       <c r="C30">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D30">
-        <v>16.45569620253164</v>
+        <v>8.860759493670885</v>
       </c>
       <c r="E30">
         <v>32</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30">
-        <v>12.65822784810127</v>
+        <v>11.39240506329114</v>
       </c>
       <c r="H30">
         <v>55</v>
@@ -38826,19 +38826,19 @@
         <v>57</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E34">
         <v>12</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H34">
         <v>36</v>
@@ -38949,10 +38949,10 @@
         <v>24</v>
       </c>
       <c r="F37">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G37">
-        <v>16.45569620253164</v>
+        <v>12.65822784810127</v>
       </c>
       <c r="H37">
         <v>47</v>
@@ -38978,19 +38978,19 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D38">
-        <v>22.36842105263158</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E38">
         <v>26</v>
       </c>
       <c r="F38">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G38">
-        <v>72.36842105263158</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H38">
         <v>75</v>
@@ -39101,10 +39101,10 @@
         <v>14</v>
       </c>
       <c r="F41">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G41">
-        <v>14.47368421052632</v>
+        <v>11.84210526315789</v>
       </c>
       <c r="H41">
         <v>49</v>
@@ -39130,19 +39130,19 @@
         <v>22</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H42">
         <v>28</v>
@@ -39168,19 +39168,19 @@
         <v>37</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D43">
-        <v>9.210526315789473</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E43">
         <v>12</v>
       </c>
       <c r="F43">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G43">
-        <v>14.47368421052632</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="H43">
         <v>57</v>
@@ -39244,10 +39244,10 @@
         <v>57</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E45">
         <v>24</v>
@@ -39443,10 +39443,10 @@
         <v>2</v>
       </c>
       <c r="F50">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G50">
-        <v>11.84210526315789</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H50">
         <v>47</v>
@@ -39481,10 +39481,10 @@
         <v>11</v>
       </c>
       <c r="F51">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G51">
-        <v>13.1578947368421</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H51">
         <v>34</v>
@@ -40013,10 +40013,10 @@
         <v>26</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G65">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H65">
         <v>28</v>
@@ -40130,10 +40130,10 @@
         <v>26</v>
       </c>
       <c r="F68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G68">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H68">
         <v>28</v>
@@ -40197,19 +40197,19 @@
         <v>85</v>
       </c>
       <c r="C70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="G70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="H70">
         <v>54</v>
@@ -40441,13 +40441,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -40631,19 +40631,19 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>76.31578947368422</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>76.31578947368422</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H7">
         <v>70</v>
@@ -40783,19 +40783,19 @@
         <v>31</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>9.210526315789473</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E11">
         <v>26</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H11">
         <v>52</v>
@@ -40973,10 +40973,10 @@
         <v>41</v>
       </c>
       <c r="C16">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>11.84210526315789</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E16">
         <v>24</v>
@@ -41087,19 +41087,19 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>76.31578947368422</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>76.31578947368422</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H19">
         <v>70</v>
@@ -41125,19 +41125,19 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D20">
-        <v>18.42105263157895</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E20">
         <v>26</v>
       </c>
       <c r="F20">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="G20">
-        <v>69.73684210526315</v>
+        <v>17.10526315789474</v>
       </c>
       <c r="H20">
         <v>75</v>
@@ -41242,19 +41242,19 @@
         <v>20</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E23">
         <v>12</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H23">
         <v>34</v>
@@ -41289,10 +41289,10 @@
         <v>17</v>
       </c>
       <c r="F24">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G24">
-        <v>17.72151898734177</v>
+        <v>10.12658227848101</v>
       </c>
       <c r="H24">
         <v>47</v>
@@ -41318,19 +41318,19 @@
         <v>41</v>
       </c>
       <c r="C25">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D25">
-        <v>11.84210526315789</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <v>11.84210526315789</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H25">
         <v>48</v>
@@ -41432,19 +41432,19 @@
         <v>24</v>
       </c>
       <c r="C28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="H28">
         <v>70</v>
@@ -41508,19 +41508,19 @@
         <v>61</v>
       </c>
       <c r="C30">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D30">
-        <v>20.25316455696203</v>
+        <v>8.860759493670885</v>
       </c>
       <c r="E30">
         <v>32</v>
       </c>
       <c r="F30">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G30">
-        <v>17.72151898734177</v>
+        <v>11.39240506329114</v>
       </c>
       <c r="H30">
         <v>55</v>
@@ -41660,19 +41660,19 @@
         <v>57</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E34">
         <v>12</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H34">
         <v>36</v>
@@ -41783,10 +41783,10 @@
         <v>24</v>
       </c>
       <c r="F37">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G37">
-        <v>18.9873417721519</v>
+        <v>12.65822784810127</v>
       </c>
       <c r="H37">
         <v>47</v>
@@ -41812,19 +41812,19 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>18.42105263157895</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E38">
         <v>26</v>
       </c>
       <c r="F38">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="G38">
-        <v>69.73684210526315</v>
+        <v>17.10526315789474</v>
       </c>
       <c r="H38">
         <v>75</v>
@@ -41926,19 +41926,19 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41">
-        <v>13.1578947368421</v>
+        <v>10.52631578947368</v>
       </c>
       <c r="E41">
         <v>14</v>
       </c>
       <c r="F41">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G41">
-        <v>14.47368421052632</v>
+        <v>11.84210526315789</v>
       </c>
       <c r="H41">
         <v>49</v>
@@ -41964,19 +41964,19 @@
         <v>22</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H42">
         <v>28</v>
@@ -42002,19 +42002,19 @@
         <v>37</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D43">
-        <v>9.210526315789473</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E43">
         <v>12</v>
       </c>
       <c r="F43">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G43">
-        <v>14.47368421052632</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="H43">
         <v>57</v>
@@ -42078,19 +42078,19 @@
         <v>57</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E45">
         <v>24</v>
       </c>
       <c r="F45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G45">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H45">
         <v>26</v>
@@ -42230,10 +42230,10 @@
         <v>83</v>
       </c>
       <c r="C49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>11.84210526315789</v>
+        <v>9.210526315789473</v>
       </c>
       <c r="E49">
         <v>11</v>
@@ -42277,10 +42277,10 @@
         <v>2</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G50">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H50">
         <v>47</v>
@@ -42315,10 +42315,10 @@
         <v>11</v>
       </c>
       <c r="F51">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G51">
-        <v>13.1578947368421</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H51">
         <v>34</v>
@@ -42847,10 +42847,10 @@
         <v>26</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G65">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H65">
         <v>28</v>
@@ -42964,10 +42964,10 @@
         <v>26</v>
       </c>
       <c r="F68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G68">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H68">
         <v>28</v>
@@ -43031,19 +43031,19 @@
         <v>85</v>
       </c>
       <c r="C70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="G70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="H70">
         <v>54</v>
@@ -43069,10 +43069,10 @@
         <v>106</v>
       </c>
       <c r="C71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D71">
-        <v>2.631578947368421</v>
+        <v>1.31578947368421</v>
       </c>
       <c r="E71">
         <v>26</v>
@@ -43107,10 +43107,10 @@
         <v>31</v>
       </c>
       <c r="C72">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D72">
-        <v>9.210526315789473</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E72">
         <v>22</v>
@@ -43275,13 +43275,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -46109,13 +46109,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -47404,19 +47404,19 @@
         <v>69</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>2.631578947368421</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E36">
         <v>34</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G36">
-        <v>2.631578947368421</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -48943,13 +48943,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -49133,19 +49133,19 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H7">
         <v>70</v>
@@ -49294,10 +49294,10 @@
         <v>26</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H11">
         <v>52</v>
@@ -49475,10 +49475,10 @@
         <v>41</v>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>10.52631578947368</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E16">
         <v>24</v>
@@ -49589,19 +49589,19 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H19">
         <v>70</v>
@@ -49627,19 +49627,19 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D20">
-        <v>22.36842105263158</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E20">
         <v>26</v>
       </c>
       <c r="F20">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G20">
-        <v>72.36842105263158</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H20">
         <v>75</v>
@@ -49744,19 +49744,19 @@
         <v>20</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E23">
         <v>12</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H23">
         <v>34</v>
@@ -49791,10 +49791,10 @@
         <v>17</v>
       </c>
       <c r="F24">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G24">
-        <v>12.65822784810127</v>
+        <v>10.12658227848101</v>
       </c>
       <c r="H24">
         <v>47</v>
@@ -49820,19 +49820,19 @@
         <v>41</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H25">
         <v>48</v>
@@ -49934,19 +49934,19 @@
         <v>24</v>
       </c>
       <c r="C28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="H28">
         <v>70</v>
@@ -50010,19 +50010,19 @@
         <v>61</v>
       </c>
       <c r="C30">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D30">
-        <v>16.45569620253164</v>
+        <v>8.860759493670885</v>
       </c>
       <c r="E30">
         <v>32</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30">
-        <v>12.65822784810127</v>
+        <v>11.39240506329114</v>
       </c>
       <c r="H30">
         <v>55</v>
@@ -50162,19 +50162,19 @@
         <v>57</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E34">
         <v>12</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H34">
         <v>36</v>
@@ -50285,10 +50285,10 @@
         <v>24</v>
       </c>
       <c r="F37">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G37">
-        <v>16.45569620253164</v>
+        <v>12.65822784810127</v>
       </c>
       <c r="H37">
         <v>47</v>
@@ -50314,19 +50314,19 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D38">
-        <v>22.36842105263158</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E38">
         <v>26</v>
       </c>
       <c r="F38">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G38">
-        <v>72.36842105263158</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H38">
         <v>75</v>
@@ -50437,10 +50437,10 @@
         <v>14</v>
       </c>
       <c r="F41">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G41">
-        <v>14.47368421052632</v>
+        <v>11.84210526315789</v>
       </c>
       <c r="H41">
         <v>49</v>
@@ -50466,19 +50466,19 @@
         <v>22</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H42">
         <v>28</v>
@@ -50504,19 +50504,19 @@
         <v>37</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D43">
-        <v>9.210526315789473</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E43">
         <v>12</v>
       </c>
       <c r="F43">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G43">
-        <v>14.47368421052632</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="H43">
         <v>57</v>
@@ -50580,10 +50580,10 @@
         <v>57</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E45">
         <v>24</v>
@@ -50779,10 +50779,10 @@
         <v>2</v>
       </c>
       <c r="F50">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G50">
-        <v>11.84210526315789</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H50">
         <v>47</v>
@@ -50817,10 +50817,10 @@
         <v>11</v>
       </c>
       <c r="F51">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G51">
-        <v>13.1578947368421</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H51">
         <v>34</v>
@@ -51349,10 +51349,10 @@
         <v>26</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G65">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H65">
         <v>28</v>
@@ -51466,10 +51466,10 @@
         <v>26</v>
       </c>
       <c r="F68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G68">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H68">
         <v>28</v>
@@ -51533,19 +51533,19 @@
         <v>85</v>
       </c>
       <c r="C70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="G70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="H70">
         <v>54</v>
@@ -51777,13 +51777,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -51967,19 +51967,19 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>76.31578947368422</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>76.31578947368422</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H7">
         <v>66</v>
@@ -52423,19 +52423,19 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>76.31578947368422</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>76.31578947368422</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H19">
         <v>66</v>
@@ -52461,19 +52461,19 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D20">
-        <v>18.42105263157895</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="E20">
         <v>26</v>
       </c>
       <c r="F20">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="G20">
-        <v>67.10526315789474</v>
+        <v>31.57894736842105</v>
       </c>
       <c r="H20">
         <v>72</v>
@@ -52768,19 +52768,19 @@
         <v>24</v>
       </c>
       <c r="C28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="H28">
         <v>66</v>
@@ -53081,10 +53081,10 @@
         <v>34</v>
       </c>
       <c r="F36">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G36">
-        <v>5.263157894736842</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -53148,19 +53148,19 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D38">
-        <v>18.42105263157895</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="E38">
         <v>26</v>
       </c>
       <c r="F38">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="G38">
-        <v>67.10526315789474</v>
+        <v>31.57894736842105</v>
       </c>
       <c r="H38">
         <v>72</v>
@@ -53452,10 +53452,10 @@
         <v>48</v>
       </c>
       <c r="C46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D46">
-        <v>5.263157894736842</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E46">
         <v>34</v>
@@ -54367,19 +54367,19 @@
         <v>85</v>
       </c>
       <c r="C70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="G70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="H70">
         <v>47</v>
@@ -54611,13 +54611,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -56818,10 +56818,10 @@
         <v>27</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D60">
-        <v>6.578947368421052</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E60">
         <v>26</v>
@@ -57445,13 +57445,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -59234,10 +59234,10 @@
         <v>83</v>
       </c>
       <c r="C49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>11.84210526315789</v>
+        <v>9.210526315789473</v>
       </c>
       <c r="E49">
         <v>11</v>
@@ -59576,19 +59576,19 @@
         <v>57</v>
       </c>
       <c r="C58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D58">
-        <v>5.263157894736842</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E58">
         <v>23</v>
       </c>
       <c r="F58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G58">
-        <v>5.263157894736842</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="H58">
         <v>5</v>
@@ -59652,10 +59652,10 @@
         <v>27</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D60">
-        <v>6.578947368421052</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E60">
         <v>26</v>
@@ -60279,13 +60279,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -60963,10 +60963,10 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D20">
-        <v>10.52631578947368</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E20">
         <v>26</v>
@@ -61650,10 +61650,10 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>10.52631578947368</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E38">
         <v>26</v>
@@ -61764,10 +61764,10 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41">
-        <v>13.1578947368421</v>
+        <v>10.52631578947368</v>
       </c>
       <c r="E41">
         <v>14</v>
@@ -63113,13 +63113,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -64598,10 +64598,10 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D41">
-        <v>15.78947368421053</v>
+        <v>10.52631578947368</v>
       </c>
       <c r="E41">
         <v>14</v>
@@ -64902,10 +64902,10 @@
         <v>83</v>
       </c>
       <c r="C49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>11.84210526315789</v>
+        <v>9.210526315789473</v>
       </c>
       <c r="E49">
         <v>11</v>
@@ -65947,13 +65947,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -67432,10 +67432,10 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41">
-        <v>13.1578947368421</v>
+        <v>10.52631578947368</v>
       </c>
       <c r="E41">
         <v>14</v>
@@ -67736,10 +67736,10 @@
         <v>83</v>
       </c>
       <c r="C49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D49">
-        <v>11.84210526315789</v>
+        <v>9.210526315789473</v>
       </c>
       <c r="E49">
         <v>11</v>
@@ -68781,13 +68781,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>10.12658227848101</v>
+        <v>8.860759493670885</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>8</v>
@@ -68819,19 +68819,19 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>2.631578947368421</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E3">
         <v>40</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>3.947368421052631</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H3">
         <v>21</v>
@@ -70380,19 +70380,19 @@
         <v>16</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>2.631578947368421</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E44">
         <v>42</v>
       </c>
       <c r="F44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G44">
-        <v>3.947368421052631</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H44">
         <v>22</v>
@@ -70912,10 +70912,10 @@
         <v>57</v>
       </c>
       <c r="C58">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D58">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E58">
         <v>23</v>
@@ -71615,13 +71615,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -73746,19 +73746,19 @@
         <v>57</v>
       </c>
       <c r="C58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D58">
-        <v>5.263157894736842</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="E58">
         <v>23</v>
       </c>
       <c r="F58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G58">
-        <v>5.263157894736842</v>
+        <v>3.947368421052631</v>
       </c>
       <c r="H58">
         <v>4</v>
@@ -74449,13 +74449,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D2">
-        <v>24.05063291139241</v>
+        <v>6.329113924050633</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>19</v>
@@ -77283,13 +77283,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -77473,19 +77473,19 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H7">
         <v>70</v>
@@ -77634,10 +77634,10 @@
         <v>26</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H11">
         <v>52</v>
@@ -77815,10 +77815,10 @@
         <v>41</v>
       </c>
       <c r="C16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>10.52631578947368</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E16">
         <v>24</v>
@@ -77929,19 +77929,19 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H19">
         <v>70</v>
@@ -77967,19 +77967,19 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D20">
-        <v>22.36842105263158</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E20">
         <v>26</v>
       </c>
       <c r="F20">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G20">
-        <v>72.36842105263158</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H20">
         <v>75</v>
@@ -78084,19 +78084,19 @@
         <v>20</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E23">
         <v>12</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H23">
         <v>34</v>
@@ -78131,10 +78131,10 @@
         <v>17</v>
       </c>
       <c r="F24">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G24">
-        <v>12.65822784810127</v>
+        <v>10.12658227848101</v>
       </c>
       <c r="H24">
         <v>47</v>
@@ -78160,19 +78160,19 @@
         <v>41</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H25">
         <v>48</v>
@@ -78274,19 +78274,19 @@
         <v>24</v>
       </c>
       <c r="C28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="H28">
         <v>70</v>
@@ -78350,19 +78350,19 @@
         <v>61</v>
       </c>
       <c r="C30">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D30">
-        <v>16.45569620253164</v>
+        <v>8.860759493670885</v>
       </c>
       <c r="E30">
         <v>32</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30">
-        <v>12.65822784810127</v>
+        <v>11.39240506329114</v>
       </c>
       <c r="H30">
         <v>55</v>
@@ -78502,19 +78502,19 @@
         <v>57</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E34">
         <v>12</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H34">
         <v>36</v>
@@ -78625,10 +78625,10 @@
         <v>24</v>
       </c>
       <c r="F37">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G37">
-        <v>16.45569620253164</v>
+        <v>12.65822784810127</v>
       </c>
       <c r="H37">
         <v>47</v>
@@ -78654,19 +78654,19 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D38">
-        <v>22.36842105263158</v>
+        <v>30.26315789473684</v>
       </c>
       <c r="E38">
         <v>26</v>
       </c>
       <c r="F38">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="G38">
-        <v>72.36842105263158</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H38">
         <v>75</v>
@@ -78777,10 +78777,10 @@
         <v>14</v>
       </c>
       <c r="F41">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G41">
-        <v>14.47368421052632</v>
+        <v>11.84210526315789</v>
       </c>
       <c r="H41">
         <v>49</v>
@@ -78806,19 +78806,19 @@
         <v>22</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H42">
         <v>28</v>
@@ -78844,19 +78844,19 @@
         <v>37</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D43">
-        <v>9.210526315789473</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E43">
         <v>12</v>
       </c>
       <c r="F43">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G43">
-        <v>14.47368421052632</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="H43">
         <v>57</v>
@@ -78920,10 +78920,10 @@
         <v>57</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E45">
         <v>24</v>
@@ -79119,10 +79119,10 @@
         <v>2</v>
       </c>
       <c r="F50">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G50">
-        <v>11.84210526315789</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H50">
         <v>47</v>
@@ -79157,10 +79157,10 @@
         <v>11</v>
       </c>
       <c r="F51">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G51">
-        <v>13.1578947368421</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H51">
         <v>34</v>
@@ -79689,10 +79689,10 @@
         <v>26</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G65">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H65">
         <v>28</v>
@@ -79806,10 +79806,10 @@
         <v>26</v>
       </c>
       <c r="F68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G68">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H68">
         <v>28</v>
@@ -79873,19 +79873,19 @@
         <v>85</v>
       </c>
       <c r="C70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="G70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="H70">
         <v>54</v>
@@ -80117,13 +80117,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -80307,19 +80307,19 @@
         <v>24</v>
       </c>
       <c r="C7">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H7">
         <v>70</v>
@@ -80468,10 +80468,10 @@
         <v>26</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11">
-        <v>9.210526315789473</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H11">
         <v>52</v>
@@ -80649,10 +80649,10 @@
         <v>41</v>
       </c>
       <c r="C16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>7.894736842105263</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E16">
         <v>24</v>
@@ -80763,19 +80763,19 @@
         <v>46</v>
       </c>
       <c r="C19">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G19">
-        <v>77.63157894736842</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="H19">
         <v>70</v>
@@ -80810,10 +80810,10 @@
         <v>26</v>
       </c>
       <c r="F20">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="G20">
-        <v>75</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H20">
         <v>75</v>
@@ -80918,19 +80918,19 @@
         <v>20</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E23">
         <v>12</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23">
-        <v>6.578947368421052</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H23">
         <v>34</v>
@@ -80965,10 +80965,10 @@
         <v>17</v>
       </c>
       <c r="F24">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G24">
-        <v>17.72151898734177</v>
+        <v>10.12658227848101</v>
       </c>
       <c r="H24">
         <v>47</v>
@@ -80994,19 +80994,19 @@
         <v>41</v>
       </c>
       <c r="C25">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D25">
-        <v>11.84210526315789</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G25">
-        <v>11.84210526315789</v>
+        <v>7.894736842105263</v>
       </c>
       <c r="H25">
         <v>48</v>
@@ -81108,19 +81108,19 @@
         <v>24</v>
       </c>
       <c r="C28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="G28">
-        <v>55.26315789473685</v>
+        <v>27.63157894736842</v>
       </c>
       <c r="H28">
         <v>70</v>
@@ -81184,10 +81184,10 @@
         <v>61</v>
       </c>
       <c r="C30">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D30">
-        <v>13.92405063291139</v>
+        <v>8.860759493670885</v>
       </c>
       <c r="E30">
         <v>32</v>
@@ -81336,19 +81336,19 @@
         <v>57</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E34">
         <v>12</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G34">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H34">
         <v>36</v>
@@ -81459,10 +81459,10 @@
         <v>24</v>
       </c>
       <c r="F37">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G37">
-        <v>16.45569620253164</v>
+        <v>12.65822784810127</v>
       </c>
       <c r="H37">
         <v>47</v>
@@ -81497,10 +81497,10 @@
         <v>26</v>
       </c>
       <c r="F38">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="G38">
-        <v>75</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="H38">
         <v>75</v>
@@ -81611,10 +81611,10 @@
         <v>14</v>
       </c>
       <c r="F41">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G41">
-        <v>14.47368421052632</v>
+        <v>11.84210526315789</v>
       </c>
       <c r="H41">
         <v>49</v>
@@ -81640,19 +81640,19 @@
         <v>22</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G42">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H42">
         <v>28</v>
@@ -81678,19 +81678,19 @@
         <v>37</v>
       </c>
       <c r="C43">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D43">
-        <v>9.210526315789473</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="E43">
         <v>12</v>
       </c>
       <c r="F43">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G43">
-        <v>14.47368421052632</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="H43">
         <v>57</v>
@@ -81754,10 +81754,10 @@
         <v>57</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="E45">
         <v>24</v>
@@ -81953,10 +81953,10 @@
         <v>2</v>
       </c>
       <c r="F50">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G50">
-        <v>11.84210526315789</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H50">
         <v>47</v>
@@ -81991,10 +81991,10 @@
         <v>11</v>
       </c>
       <c r="F51">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G51">
-        <v>13.1578947368421</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="H51">
         <v>34</v>
@@ -82523,10 +82523,10 @@
         <v>26</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G65">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H65">
         <v>28</v>
@@ -82640,10 +82640,10 @@
         <v>26</v>
       </c>
       <c r="F68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G68">
-        <v>3.947368421052631</v>
+        <v>2.631578947368421</v>
       </c>
       <c r="H68">
         <v>28</v>
@@ -82707,19 +82707,19 @@
         <v>85</v>
       </c>
       <c r="C70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="G70">
-        <v>51.31578947368421</v>
+        <v>23.68421052631579</v>
       </c>
       <c r="H70">
         <v>54</v>
@@ -82783,10 +82783,10 @@
         <v>31</v>
       </c>
       <c r="C72">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D72">
-        <v>9.210526315789473</v>
+        <v>6.578947368421052</v>
       </c>
       <c r="E72">
         <v>22</v>
@@ -82951,13 +82951,13 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2">
-        <v>8.860759493670885</v>
+        <v>7.59493670886076</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>7</v>
@@ -83635,10 +83635,10 @@
         <v>48</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D20">
-        <v>11.84210526315789</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E20">
         <v>26</v>
@@ -84322,10 +84322,10 @@
         <v>16</v>
       </c>
       <c r="C38">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>11.84210526315789</v>
+        <v>14.47368421052632</v>
       </c>
       <c r="E38">
         <v>26</v>
@@ -84436,10 +84436,10 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D41">
-        <v>13.1578947368421</v>
+        <v>10.52631578947368</v>
       </c>
       <c r="E41">
         <v>14</v>

</xml_diff>